<commit_message>
Added training ground model seeding with fixed 10 entries
</commit_message>
<xml_diff>
--- a/tactera_backend/xp_levels.xlsx
+++ b/tactera_backend/xp_levels.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbusP\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbusP\Tactera\tactera_backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB7491B7-A528-4EC2-BA4A-53A5FC1E12B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D6084F-E8D3-4F08-BC1E-5BBCAE97691E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0645EBBE-6A6B-463A-A126-B7FCA025158C}"/>
+    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11295" xr2:uid="{0645EBBE-6A6B-463A-A126-B7FCA025158C}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -417,7 +417,7 @@
   <dimension ref="A1:B252"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -437,6 +437,9 @@
       <c r="A2">
         <v>1</v>
       </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">

</xml_diff>

<commit_message>
Updated XP levels seeding to read from CSV file with all 251 levels
- Modified seed_xp_levels.py to read from xp_levels.csv instead of programmatic generation
- Added support for semicolon-delimited CSV format (Level;Accumulated xp)
- Added fallback function that approximates CSV progression if file loading fails
- Now processes all 251 rows instead of being limited to 50 rows
- Improved error handling and logging for CSV processing
- Added xp_levels.csv with complete level progression (1-250)
</commit_message>
<xml_diff>
--- a/tactera_backend/xp_levels.xlsx
+++ b/tactera_backend/xp_levels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AbusP\Tactera\tactera_backend\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63D6084F-E8D3-4F08-BC1E-5BBCAE97691E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B21514-5BC5-43AA-823B-47E8C49D31B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1905" yWindow="1905" windowWidth="21600" windowHeight="11295" xr2:uid="{0645EBBE-6A6B-463A-A126-B7FCA025158C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{0645EBBE-6A6B-463A-A126-B7FCA025158C}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -416,7 +416,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1845E6EC-2D9B-4943-8A30-9ABD286AF937}">
   <dimension ref="A1:B252"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>

</xml_diff>